<commit_message>
Politica adattativa - inizio test
</commit_message>
<xml_diff>
--- a/Statistiche/tablet/dati consumi.xlsx
+++ b/Statistiche/tablet/dati consumi.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Telefono" sheetId="1" r:id="rId1"/>
     <sheet name="Tablet" sheetId="2" r:id="rId2"/>
     <sheet name="Tab2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,8 +104,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +170,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -268,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -325,7 +331,17 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
@@ -346,26 +362,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -541,7 +537,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2072-4EFA-A086-D503856CA988}"/>
             </c:ext>
@@ -555,11 +551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="304393368"/>
-        <c:axId val="304392712"/>
+        <c:axId val="177406720"/>
+        <c:axId val="177408256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="304393368"/>
+        <c:axId val="177406720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,12 +612,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304392712"/>
+        <c:crossAx val="177408256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="304392712"/>
+        <c:axId val="177408256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +674,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304393368"/>
+        <c:crossAx val="177406720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -728,7 +724,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -772,7 +768,17 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT" sz="1800" b="0" i="0" baseline="0">
@@ -792,26 +798,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -999,7 +985,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-199F-4434-B17A-207DB1DC30D7}"/>
             </c:ext>
@@ -1013,11 +999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="308336656"/>
-        <c:axId val="308335672"/>
+        <c:axId val="177437696"/>
+        <c:axId val="177464064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="308336656"/>
+        <c:axId val="177437696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,12 +1060,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308335672"/>
+        <c:crossAx val="177464064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="308335672"/>
+        <c:axId val="177464064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1122,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308336656"/>
+        <c:crossAx val="177437696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1186,7 +1172,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -1224,12 +1210,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="it-IT" baseline="0"/>
-              <a:t> pull 5 sec</a:t>
+              <a:t> pull ogni 5 sec</a:t>
             </a:r>
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1238,26 +1225,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1391,43 +1358,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A5D-4E89-8DEC-DB295FEDB351}"/>
             </c:ext>
@@ -1441,11 +1408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297702736"/>
-        <c:axId val="297704048"/>
+        <c:axId val="177678208"/>
+        <c:axId val="177679744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297702736"/>
+        <c:axId val="177678208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,6 +1432,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> [sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1502,12 +1493,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297704048"/>
+        <c:crossAx val="177679744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297704048"/>
+        <c:axId val="177679744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,6 +1518,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>livello batteria</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1564,7 +1574,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297702736"/>
+        <c:crossAx val="177678208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,7 +1624,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -1648,11 +1658,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>1 pull 1 sec</a:t>
+              <a:t>1 pull al sec</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1661,26 +1672,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1814,43 +1805,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>71</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>70</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-66F7-4742-B1C0-29DCF41F7830}"/>
             </c:ext>
@@ -1864,11 +1855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297694536"/>
-        <c:axId val="297699128"/>
+        <c:axId val="177725824"/>
+        <c:axId val="177727360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297694536"/>
+        <c:axId val="177725824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,6 +1879,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>tempo [sec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1925,12 +1935,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297699128"/>
+        <c:crossAx val="177727360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297699128"/>
+        <c:axId val="177727360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,6 +1960,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>livello batteria</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1987,7 +2016,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297694536"/>
+        <c:crossAx val="177725824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2037,7 +2066,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -2075,11 +2104,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="it-IT" baseline="0"/>
-              <a:t> pull 10 sec</a:t>
+              <a:t> pull ogni 10 sec</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2088,26 +2118,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2241,43 +2251,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ECCA-4DF8-897A-6BBB0D41B849}"/>
             </c:ext>
@@ -2291,11 +2301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299116560"/>
-        <c:axId val="299110656"/>
+        <c:axId val="177824128"/>
+        <c:axId val="177825664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299116560"/>
+        <c:axId val="177824128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,6 +2325,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> [sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2352,12 +2386,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299110656"/>
+        <c:crossAx val="177825664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299110656"/>
+        <c:axId val="177825664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,6 +2411,25 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>livello batteria</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2414,7 +2467,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299116560"/>
+        <c:crossAx val="177824128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2464,7 +2517,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -2498,11 +2551,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>1 pull 20 sec</a:t>
+              <a:t>1 pull ogni 20 sec</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2511,26 +2565,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2700,7 +2734,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3E81-4ED2-B724-B5C914F8ABAD}"/>
             </c:ext>
@@ -2714,11 +2748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306801360"/>
-        <c:axId val="306799720"/>
+        <c:axId val="177863680"/>
+        <c:axId val="177865472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306801360"/>
+        <c:axId val="177863680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,6 +2772,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> [sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2775,12 +2833,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306799720"/>
+        <c:crossAx val="177865472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306799720"/>
+        <c:axId val="177865472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2800,6 +2858,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>livello</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> batteria</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2837,7 +2919,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306801360"/>
+        <c:crossAx val="177863680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2887,7 +2969,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -2901,6 +2983,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Velocità media di scarica</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2909,26 +3017,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3065,7 +3153,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F537-4DD4-ACD0-320D8B0611BE}"/>
             </c:ext>
@@ -3079,11 +3167,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="244658520"/>
-        <c:axId val="244660488"/>
+        <c:axId val="177909760"/>
+        <c:axId val="177911296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="244658520"/>
+        <c:axId val="177909760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,6 +3191,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>frequenza</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> di pull [pull/sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3140,12 +3252,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244660488"/>
+        <c:crossAx val="177911296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244660488"/>
+        <c:axId val="177911296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,6 +3277,30 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>velocità</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" baseline="0"/>
+                  <a:t> media scarica</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3202,7 +3338,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244658520"/>
+        <c:crossAx val="177909760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3252,7 +3388,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -3291,6 +3427,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3299,26 +3436,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3488,7 +3605,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AAFF-41AA-B96F-17F6EDF8E8FE}"/>
             </c:ext>
@@ -3502,11 +3619,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="395416152"/>
-        <c:axId val="395418776"/>
+        <c:axId val="177953024"/>
+        <c:axId val="177975296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="395416152"/>
+        <c:axId val="177953024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3563,12 +3680,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395418776"/>
+        <c:crossAx val="177975296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="395418776"/>
+        <c:axId val="177975296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3625,7 +3742,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395416152"/>
+        <c:crossAx val="177953024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8142,7 +8259,7 @@
         <xdr:cNvPr id="2" name="Grafico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2FA714D-01FA-45DF-8D0D-00BF5A75AC93}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2FA714D-01FA-45DF-8D0D-00BF5A75AC93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8178,7 +8295,7 @@
         <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1291D28D-6725-4D1E-B13F-4FC55E3CC6EE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1291D28D-6725-4D1E-B13F-4FC55E3CC6EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8219,7 +8336,7 @@
         <xdr:cNvPr id="2" name="Grafico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C32D2E-9A65-4567-8287-03C1584B9F91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C32D2E-9A65-4567-8287-03C1584B9F91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8255,7 +8372,7 @@
         <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AF724F6-D994-4252-8CA4-084BEF714D15}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AF724F6-D994-4252-8CA4-084BEF714D15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8291,7 +8408,7 @@
         <xdr:cNvPr id="4" name="Grafico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BB4DDE-3D07-482B-886B-F280EF59D9E4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BB4DDE-3D07-482B-886B-F280EF59D9E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8327,7 +8444,7 @@
         <xdr:cNvPr id="5" name="Grafico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590FE9A2-38E3-4589-AA45-7E9E4B9E4A6D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590FE9A2-38E3-4589-AA45-7E9E4B9E4A6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8363,7 +8480,7 @@
         <xdr:cNvPr id="7" name="Grafico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9754E5-50FF-4E0A-8AFE-711DC3563B27}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9754E5-50FF-4E0A-8AFE-711DC3563B27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8404,7 +8521,7 @@
         <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A92E5C9C-B7BB-4588-8B87-F6FB88996906}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A92E5C9C-B7BB-4588-8B87-F6FB88996906}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8423,110 +8540,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Telefono"/>
-      <sheetName val="Tablet"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="68">
-          <cell r="C68">
-            <v>0</v>
-          </cell>
-          <cell r="D68">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>1794</v>
-          </cell>
-          <cell r="D69">
-            <v>99</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>2479</v>
-          </cell>
-          <cell r="D70">
-            <v>98</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>2844</v>
-          </cell>
-          <cell r="D71">
-            <v>97</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>3313</v>
-          </cell>
-          <cell r="D72">
-            <v>96</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>3872</v>
-          </cell>
-          <cell r="D73">
-            <v>95</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>4644</v>
-          </cell>
-          <cell r="D74">
-            <v>94</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>4836</v>
-          </cell>
-          <cell r="D75">
-            <v>93</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>5325</v>
-          </cell>
-          <cell r="D76">
-            <v>92</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>5795</v>
-          </cell>
-          <cell r="D77">
-            <v>91</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>6444</v>
-          </cell>
-          <cell r="D78">
-            <v>90</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8572,7 +8585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -8607,7 +8620,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -8784,7 +8797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9263,10 +9276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E89"/>
+  <dimension ref="A2:O89"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9299,7 +9312,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -9315,7 +9328,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:D13" si="1">D3-1</f>
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -9331,7 +9344,7 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -9347,7 +9360,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -9363,7 +9376,7 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -9379,7 +9392,7 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -9395,7 +9408,7 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -9411,7 +9424,7 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -9427,7 +9440,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -9443,7 +9456,7 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -9459,7 +9472,7 @@
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -9489,7 +9502,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>4</v>
       </c>
@@ -9504,7 +9517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>9</v>
       </c>
@@ -9520,10 +9533,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>19</v>
       </c>
@@ -9540,10 +9553,10 @@
       </c>
       <c r="E19" s="3">
         <f t="shared" ref="E19:E28" si="4">E18-1</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>28</v>
       </c>
@@ -9560,10 +9573,10 @@
       </c>
       <c r="E20" s="3">
         <f t="shared" si="4"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>36</v>
       </c>
@@ -9580,10 +9593,10 @@
       </c>
       <c r="E21" s="3">
         <f t="shared" si="4"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>44</v>
       </c>
@@ -9600,10 +9613,10 @@
       </c>
       <c r="E22" s="3">
         <f t="shared" si="4"/>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>53</v>
       </c>
@@ -9620,10 +9633,10 @@
       </c>
       <c r="E23" s="3">
         <f t="shared" si="4"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>62</v>
       </c>
@@ -9640,10 +9653,10 @@
       </c>
       <c r="E24" s="3">
         <f t="shared" si="4"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>68</v>
       </c>
@@ -9660,10 +9673,10 @@
       </c>
       <c r="E25" s="3">
         <f t="shared" si="4"/>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>77</v>
       </c>
@@ -9680,10 +9693,10 @@
       </c>
       <c r="E26" s="3">
         <f t="shared" si="4"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>84</v>
       </c>
@@ -9700,10 +9713,10 @@
       </c>
       <c r="E27" s="3">
         <f t="shared" si="4"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>93</v>
       </c>
@@ -9720,10 +9733,11 @@
       </c>
       <c r="E28" s="4">
         <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="O28" s="21"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>6</v>
       </c>
@@ -9739,7 +9753,7 @@
         <v>-2.0249999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>9</v>
       </c>
@@ -9780,7 +9794,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="9">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -9800,7 +9814,7 @@
       </c>
       <c r="E35" s="9">
         <f>E34-1</f>
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -9820,7 +9834,7 @@
       </c>
       <c r="E36" s="9">
         <f>E35-1</f>
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -9840,7 +9854,7 @@
       </c>
       <c r="E37" s="9">
         <f>E36-1</f>
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -9860,7 +9874,7 @@
       </c>
       <c r="E38" s="9">
         <f t="shared" ref="E38:E44" si="7">E37-1</f>
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -9880,7 +9894,7 @@
       </c>
       <c r="E39" s="9">
         <f t="shared" si="7"/>
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -9900,7 +9914,7 @@
       </c>
       <c r="E40" s="11">
         <f t="shared" si="7"/>
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -9920,7 +9934,7 @@
       </c>
       <c r="E41" s="9">
         <f t="shared" si="7"/>
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -9940,7 +9954,7 @@
       </c>
       <c r="E42" s="9">
         <f t="shared" si="7"/>
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -9960,7 +9974,7 @@
       </c>
       <c r="E43" s="9">
         <f t="shared" si="7"/>
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -9980,7 +9994,7 @@
       </c>
       <c r="E44" s="12">
         <f t="shared" si="7"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -10371,8 +10385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>